<commit_message>
Excel hasil ouput fuzzy
</commit_message>
<xml_diff>
--- a/peringkat.xlsx
+++ b/peringkat.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,95 +422,95 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
-          <t>id Pelanggan</t>
+          <t>ID Pelanggan</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
-          <t>Pelayanan</t>
+          <t>Kualitas Servis (1-100)</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
-          <t>harga</t>
+          <t>Harga (Rp)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
-          <t>Skor Kelayakan</t>
+          <t>Skor Kelayakan (0-100)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="B2" t="n">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C2" t="n">
-        <v>24704</v>
+        <v>29811</v>
       </c>
       <c r="D2" t="n">
-        <v>90</v>
+        <v>85.40940000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>23</v>
+        <v>80</v>
       </c>
       <c r="B3" t="n">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="C3" t="n">
-        <v>22825</v>
+        <v>22012</v>
       </c>
       <c r="D3" t="n">
-        <v>90</v>
+        <v>85.40349999999999</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="B4" t="n">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C4" t="n">
-        <v>34513</v>
+        <v>22360</v>
       </c>
       <c r="D4" t="n">
-        <v>90</v>
+        <v>85.2278</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="B5" t="n">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C5" t="n">
-        <v>29803</v>
+        <v>27315</v>
       </c>
       <c r="D5" t="n">
-        <v>90</v>
+        <v>85.0582</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C6" t="n">
-        <v>39211</v>
+        <v>20052</v>
       </c>
       <c r="D6" t="n">
-        <v>90</v>
+        <v>84.70489999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>